<commit_message>
update home page and fix the project page
</commit_message>
<xml_diff>
--- a/app/projects/ProjectsTracker.xlsx
+++ b/app/projects/ProjectsTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbenc\Downloads\my-website\app\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5509394-1329-431E-887C-ADD9ABAFCD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1E04B4-7D81-43D7-99D4-B093FFDB907B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E70EA1F-4D9B-4103-BAF7-03CABB45CF40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>https://github.com/Dylan-Perrill/SternsBankHackathon</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>Computer Vision, OpenCV, Java, Image Processing</t>
+  </si>
+  <si>
+    <t>Javascript, HTML, CSS, LLM, API</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>View on Github</t>
   </si>
 </sst>
 </file>
@@ -445,53 +460,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DF0671-45F3-4F36-A529-3F64BE8A1999}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F9" s="1"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>